<commit_message>
Upload landbyregion.png test file for testing.md
</commit_message>
<xml_diff>
--- a/assets/documents/excel_files/LandByRegion.xlsx
+++ b/assets/documents/excel_files/LandByRegion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardread/Dropbox/WebPages/CodeInstitute/Milestone Project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardread/Dropbox (Personal)/WebPages/CodeInstitute/Milestone Project 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F76E51-7C50-9549-9091-AE9DDD0A8465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8781338F-C154-3742-BB4F-7A4EFC591B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LandByRegion" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
   <si>
     <t>Land area is a country's total area, excluding area under inland water bodies, national claims to continental shelf, and exclusive economic zones. In most cases the definition of inland water bodies includes major rivers and lakes.</t>
   </si>
@@ -234,7 +234,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -277,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -581,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -877,6 +877,153 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>2381740</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>995450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>446300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>1759540</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>23180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>155360</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23">
+        <f>SUM(E17:E22)</f>
+        <v>5761570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -983,7 +1130,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1137,5 +1284,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>